<commit_message>
Added engine.py fields_map and simulation.py Other changes
</commit_message>
<xml_diff>
--- a/test/file/input/control_test_1/network.xlsx
+++ b/test/file/input/control_test_1/network.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FBK106\Documents\Repositories\ResiliencyTool\file\input\Simulation_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FBK106\Documents\Repositories\ResiliencyTool\test\file\input\control_test_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C894DEF-CFD2-4787-8A0A-723027D5C81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B402425-9706-4B3D-B625-68CE4FEE0B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="12" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="165">
   <si>
     <t>name</t>
   </si>
@@ -539,6 +539,9 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>slack</t>
   </si>
 </sst>
 </file>
@@ -3944,7 +3947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA625533-3B9A-44F8-8593-9BC4C933B1AA}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -4437,8 +4440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB5B7B5-BF13-4654-A134-6B30DC3D029F}">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D1:D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4532,6 +4535,9 @@
       <c r="U1" t="s">
         <v>93</v>
       </c>
+      <c r="V1" t="s">
+        <v>164</v>
+      </c>
       <c r="W1" t="s">
         <v>3</v>
       </c>
@@ -4561,6 +4567,9 @@
       <c r="M2" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="V2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4584,6 +4593,9 @@
       <c r="M3" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="V3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -4607,6 +4619,9 @@
       <c r="M4" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="V4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -4630,6 +4645,9 @@
       <c r="M5" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="V5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -4653,6 +4671,9 @@
       <c r="M6" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="V6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -4675,6 +4696,9 @@
       </c>
       <c r="M7" s="2" t="s">
         <v>106</v>
+      </c>
+      <c r="V7" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5080,7 +5104,7 @@
       </c>
       <c r="P2">
         <f ca="1">RANDBETWEEN(0,0.8*simulation!$C$5)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -5134,7 +5158,7 @@
       </c>
       <c r="P4">
         <f ca="1">RANDBETWEEN(0,0.8*simulation!$C$5)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -5161,7 +5185,7 @@
       </c>
       <c r="P5" s="6">
         <f ca="1">RANDBETWEEN(0,0.8*simulation!$C$5)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -5188,7 +5212,7 @@
       </c>
       <c r="P6">
         <f ca="1">RANDBETWEEN(0,0.8*simulation!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -5242,7 +5266,7 @@
       </c>
       <c r="P8">
         <f ca="1">RANDBETWEEN(0,0.8*simulation!$C$5)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -5269,7 +5293,7 @@
       </c>
       <c r="P9">
         <f ca="1">RANDBETWEEN(0,0.8*simulation!$C$5)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -5323,7 +5347,7 @@
       </c>
       <c r="P11">
         <f ca="1">RANDBETWEEN(0,0.8*simulation!$C$5)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -5377,7 +5401,7 @@
       </c>
       <c r="P13">
         <f ca="1">RANDBETWEEN(0,0.8*simulation!$C$5)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -5404,7 +5428,7 @@
       </c>
       <c r="P14">
         <f ca="1">RANDBETWEEN(0,0.8*simulation!$C$5)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -5485,7 +5509,7 @@
       </c>
       <c r="P17">
         <f ca="1">RANDBETWEEN(0,0.8*simulation!$C$5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>